<commit_message>
new api adapt, problem with resource consumption
</commit_message>
<xml_diff>
--- a/Quiz_Graded.xlsx
+++ b/Quiz_Graded.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD122"/>
+  <dimension ref="A1:Y122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,47 +541,22 @@
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Reason 1</t>
+          <t>Soru 2 Puan</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Soru 2 Puan</t>
+          <t>Soru 3 Puan</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>Reason 2</t>
+          <t>Soru 4 Puan</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Soru 3 Puan</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>Reason 3</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>Soru 4 Puan</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>Reason 4</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
           <t>Soru 5 Puan</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>Reason 5</t>
         </is>
       </c>
     </row>
@@ -682,47 +657,22 @@
         </is>
       </c>
       <c r="T2" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="U2" t="n">
-        <v>10</v>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>The student correctly identified the industrial revolution and mentioned a relevant example related to chemistry patents, showing understanding of chemistry's role in innovation. However, the answer lacks the identification of a second historical milestone and the explanation of chemistry's role in it, therefore only partial points are awarded.</t>
-        </is>
+        <v>15</v>
+      </c>
+      <c r="V2" t="n">
+        <v>20</v>
       </c>
       <c r="W2" t="n">
         <v>20</v>
       </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>The student accurately explains how a common nomenclature transcends language barriers, facilitating scientific collaboration and the dissemination of knowledge. The connection between nomenclature, education, and the acceptance of scientific truths is also well-explained.</t>
-        </is>
+      <c r="X2" t="n">
+        <v>20</v>
       </c>
       <c r="Y2" t="n">
         <v>20</v>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>The student suggests two valid alternatives for innovation in chemistry: developing new measurement devices and organizing chemical groups (like the periodic table). Both suggestions demonstrate an understanding of different approaches to advancing chemical knowledge.</t>
-        </is>
-      </c>
-      <c r="AA2" t="n">
-        <v>20</v>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>The student provides a comprehensive list of pivotal instruments (analytical balance, voltaic batteries, etc.) and methods (distillation, crystallization, electrolysis) used in the development of chemistry, showcasing a strong understanding of the field's history.</t>
-        </is>
-      </c>
-      <c r="AC2" t="n">
-        <v>20</v>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>The student correctly explains the significance of Mendeleev's periodic table: organizing elements into families with similar properties, predicting undiscovered elements, and providing a more complete and accurate classification compared to previous attempts.  The answer demonstrates a thorough understanding of the periodic table's impact.</t>
-        </is>
       </c>
     </row>
     <row r="3">
@@ -821,49 +771,12 @@
           <t>20230808012</t>
         </is>
       </c>
-      <c r="T3" t="n">
-        <v>85</v>
-      </c>
-      <c r="U3" t="n">
-        <v>16</v>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>The answer correctly identifies the Scientific Revolution and the Industrial Age as key milestones and discusses the role of chemistry in both periods.  However, the explanation lacks depth and precision in some parts. For example, the explanation of the impact of nomenclature could be more detailed. The example of nylon is a bit too modern for the Industrial Age focus.</t>
-        </is>
-      </c>
-      <c r="W3" t="n">
-        <v>18</v>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student correctly defines nomenclature and explains its importance in scientific collaboration. The reference to Lavoisier adds context and shows understanding. </t>
-        </is>
-      </c>
-      <c r="Y3" t="n">
-        <v>19</v>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>The answer offers valid alternative approaches to innovation in chemistry beyond experimentation.  It correctly mentions theoretical approaches (like Dalton's work), examining existing theories from new perspectives, developing new instruments, and improving existing ones.  The explanation is well-structured and thoughtful.</t>
-        </is>
-      </c>
-      <c r="AA3" t="n">
-        <v>17</v>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>The student identifies key instruments and methods and correctly connects them to significant developments in chemistry, such as the analytical balance and conservation of mass. The mention of the spectroscope and thermometer further strengthens the response.  However, the answer lacks detailed explanations of how Jabir Ibn Hayyan's laboratory methods contributed.</t>
-        </is>
-      </c>
-      <c r="AC3" t="n">
-        <v>15</v>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>The answer correctly points out the importance of the periodic table in organizing elements and predicting their properties.  However, it is a bit brief and could benefit from more elaborate discussion of its impact on the field of chemistry.</t>
-        </is>
-      </c>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -961,49 +874,12 @@
           <t>20240808606</t>
         </is>
       </c>
-      <c r="T4" t="n">
-        <v>77</v>
-      </c>
-      <c r="U4" t="n">
-        <v>10</v>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>The student partially explained the role of alchemy in the development of chemistry and vaguely mentioned a new era in chemistry.  However, the answer lacks depth and specific examples of milestones.</t>
-        </is>
-      </c>
-      <c r="W4" t="n">
-        <v>18</v>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student correctly identifies the role of nomenclature in making science more accessible and fostering collaboration, leading to faster advancements. </t>
-        </is>
-      </c>
-      <c r="Y4" t="n">
-        <v>18</v>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student correctly points out the necessity of experiments in chemistry and suggests alternatives using mathematical models and AI for computational chemistry. The answer demonstrates a good understanding of the topic. </t>
-        </is>
-      </c>
-      <c r="AA4" t="n">
-        <v>12</v>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student lists several important instruments and methods used in chemistry, but lacks a detailed explanation of their significance and impact on the field. </t>
-        </is>
-      </c>
-      <c r="AC4" t="n">
-        <v>19</v>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student accurately describes Mendeleev's contribution, Moseley's refinement, and the significance of the periodic table in predicting missing elements and classifying elements based on their properties. </t>
-        </is>
-      </c>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1101,49 +977,12 @@
           <t>20240808612</t>
         </is>
       </c>
-      <c r="T5" t="n">
-        <v>35</v>
-      </c>
-      <c r="U5" t="n">
-        <v>10</v>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>The student partially mentions the four elements of Aristotle and some elements discovered in the 18th century, showing basic knowledge. However, the answer lacks depth and context regarding the milestones' significance.</t>
-        </is>
-      </c>
-      <c r="W5" t="n">
-        <v>5</v>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>The student vaguely mentions the usefulness of nomenclature in chemistry and science, but doesn't elaborate on how it contributes to the development of scientific knowledge, theories, or communication.</t>
-        </is>
-      </c>
-      <c r="Y5" t="n">
-        <v>5</v>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>The student suggests mathematics and physics as alternatives to experiments, which is partially correct as theoretical work is crucial.  However, the answer lacks depth and doesn't explore other potential alternatives for innovation in chemistry.</t>
-        </is>
-      </c>
-      <c r="AA5" t="n">
-        <v>10</v>
-      </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>The student mentions a balance (referencing Joseph Black) and Jabir ibn Hayyan, demonstrating some knowledge of important figures and tools. However, the answer is superficial and lacks elaboration on the pivotal role of these instruments/methods.</t>
-        </is>
-      </c>
-      <c r="AC5" t="n">
-        <v>5</v>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>The student mentions that Mendeleev discovered elements with the same quantities, which is vague. The answer fails to capture the significance of the periodic table in organizing elements and predicting properties.</t>
-        </is>
-      </c>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1241,49 +1080,12 @@
           <t>20230808016</t>
         </is>
       </c>
-      <c r="T6" t="n">
-        <v>60</v>
-      </c>
-      <c r="U6" t="n">
-        <v>10</v>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>The student partially understood the importance of chemistry in World War 2 and in disproving Aristotle's theory. However, the answer lacks specific details and historical accuracy. The connection between the Manhattan Project and the need for rapid development of chemistry is vaguely mentioned, and the explanation of the overthrow of Aristotle's theory is too simplistic.</t>
-        </is>
-      </c>
-      <c r="W6" t="n">
-        <v>10</v>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>The student correctly identified the role of nomenclature in enabling communication and collaboration among chemists.  However, the answer is too brief and doesn't elaborate on other benefits of standardized terminology.</t>
-        </is>
-      </c>
-      <c r="Y6" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>The student provided a valid alternative approach (mathematical modeling) to experimental innovation in chemistry.  The reference to Oppenheimer is relevant but could be more precise. The answer lacks further exploration of different alternative approaches.</t>
-        </is>
-      </c>
-      <c r="AA6" t="n">
-        <v>18</v>
-      </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>The student correctly identified several crucial instruments and methods in the development of chemistry, showing good knowledge of historical tools and techniques. The answer is detailed and well-structured, demonstrating a good understanding of the topic.</t>
-        </is>
-      </c>
-      <c r="AC6" t="n">
-        <v>12</v>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>The student accurately described Mendeleev's discovery of the periodic table and the key insight of predicting undiscovered elements based on recurring properties. The answer lacks depth in explaining the broader impact and significance of this discovery.</t>
-        </is>
-      </c>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1381,49 +1183,12 @@
           <t>20230808009</t>
         </is>
       </c>
-      <c r="T7" t="n">
-        <v>64</v>
-      </c>
-      <c r="U7" t="n">
-        <v>14</v>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>The student correctly identifies the shift from the four-element theory to the identification of chemical elements as a major development in the 18th century.  The mention of Lavoisier and the periodic table further strengthens the answer. However, the explanation of vitalism is inaccurate and incomplete, preventing full points.</t>
-        </is>
-      </c>
-      <c r="W7" t="n">
-        <v>10</v>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>The student demonstrates a basic understanding of the importance of nomenclature in science, but the answer lacks depth and specific examples to fully illustrate its role in scientific development.</t>
-        </is>
-      </c>
-      <c r="Y7" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>The student provides alternative methods for innovation beyond experimentation, but the response is somewhat vague and lacks specific details.  The answer touches on important aspects, like observation and prediction, but doesn't elaborate effectively.</t>
-        </is>
-      </c>
-      <c r="AA7" t="n">
-        <v>12</v>
-      </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>The student correctly identifies some crucial instruments and methods in the development of chemistry.  However, the answer would benefit from more examples and a deeper explanation of their impact.</t>
-        </is>
-      </c>
-      <c r="AC7" t="n">
-        <v>18</v>
-      </c>
-      <c r="AD7" t="inlineStr">
-        <is>
-          <t>The student accurately describes Mendeleev's contribution and the significance of the periodic table.  The explanation of its predictive power and utility is well-articulated.</t>
-        </is>
-      </c>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1521,49 +1286,12 @@
           <t>20240808508</t>
         </is>
       </c>
-      <c r="T8" t="n">
-        <v>60</v>
-      </c>
-      <c r="U8" t="n">
-        <v>10</v>
-      </c>
-      <c r="V8" t="inlineStr">
-        <is>
-          <t>The answer shows a basic understanding of chemistry's historical development, mentioning key figures and eras. However, it lacks depth in connecting these milestones to the question's prompt about foundational importance and its role as a driver of innovation.</t>
-        </is>
-      </c>
-      <c r="W8" t="n">
-        <v>12</v>
-      </c>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>The student correctly identifies Lavoisier's contribution to chemical nomenclature and makes an analogy to programming languages to illustrate the importance of standardization.  However, the explanation lacks depth in elaborating the impact on scientific collaboration and the overall development of science.</t>
-        </is>
-      </c>
-      <c r="Y8" t="n">
-        <v>8</v>
-      </c>
-      <c r="Z8" t="inlineStr">
-        <is>
-          <t>The answer suggests alternatives to conducting experiments, focusing on educational initiatives. While relevant to the advancement of chemistry, it does not directly address the question's prompt about innovation in chemistry through experimental methods.</t>
-        </is>
-      </c>
-      <c r="AA8" t="n">
-        <v>15</v>
-      </c>
-      <c r="AB8" t="inlineStr">
-        <is>
-          <t>The student lists several important instruments and methods in chemistry with brief explanations. The answer is factually correct, but it lacks discussion of their specific pivotal role in the development of chemistry.</t>
-        </is>
-      </c>
-      <c r="AC8" t="n">
-        <v>15</v>
-      </c>
-      <c r="AD8" t="inlineStr">
-        <is>
-          <t>The answer correctly points out Mendeleev's contribution to organizing elements, highlighting its predictive power and influence on future discoveries.  The answer demonstrates understanding but lacks detailed discussion of the significance.</t>
-        </is>
-      </c>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1661,49 +1389,12 @@
           <t>20230808047</t>
         </is>
       </c>
-      <c r="T9" t="n">
-        <v>78</v>
-      </c>
-      <c r="U9" t="n">
-        <v>10</v>
-      </c>
-      <c r="V9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student partially understands chemistry's historical role, mentioning both ancient and modern applications. However, the answer lacks depth in explaining the milestones and their significance. </t>
-        </is>
-      </c>
-      <c r="W9" t="n">
-        <v>18</v>
-      </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student correctly identifies the role of nomenclature in facilitating scientific collaboration and information sharing, leading to faster scientific progress.  </t>
-        </is>
-      </c>
-      <c r="Y9" t="n">
-        <v>15</v>
-      </c>
-      <c r="Z9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student correctly points out that observation is an alternative to experiments for making discoveries and improving hypotheses, illustrating with Dalton's example. </t>
-        </is>
-      </c>
-      <c r="AA9" t="n">
-        <v>16</v>
-      </c>
-      <c r="AB9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student lists several important instruments and methods in chemistry (spectroscope, thermometer, barometer, stoichiometry, radioactivity, nomenclature) and briefly describes their roles. However, some descriptions are superficial. </t>
-        </is>
-      </c>
-      <c r="AC9" t="n">
-        <v>19</v>
-      </c>
-      <c r="AD9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student correctly explains Mendeleev's organization of elements by atomic mass and properties, highlighting the prediction of missing elements. </t>
-        </is>
-      </c>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1801,49 +1492,12 @@
           <t>20230808065</t>
         </is>
       </c>
-      <c r="T10" t="n">
-        <v>81</v>
-      </c>
-      <c r="U10" t="n">
-        <v>10</v>
-      </c>
-      <c r="V10" t="inlineStr">
-        <is>
-          <t>The student partially answered the question by mentioning Aristotle's elements and the importance of nomenclature. However, they did not fully explain the significance of these milestones in driving innovation and progress.</t>
-        </is>
-      </c>
-      <c r="W10" t="n">
-        <v>18</v>
-      </c>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>The student correctly explained how nomenclature made chemistry universal and systematical, facilitating education, research, discoveries, and data transfer.  The answer is comprehensive.</t>
-        </is>
-      </c>
-      <c r="Y10" t="n">
-        <v>16</v>
-      </c>
-      <c r="Z10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student provided a valid alternative to experimental innovation through theoretical calculations and data analysis, showing good understanding of the role of theoretical chemistry. </t>
-        </is>
-      </c>
-      <c r="AA10" t="n">
-        <v>18</v>
-      </c>
-      <c r="AB10" t="inlineStr">
-        <is>
-          <t>The student accurately identified pivotal instruments and methods in chemistry's development, such as thermometers, barometers, alembics, and distillation. The answer is detailed and accurate.</t>
-        </is>
-      </c>
-      <c r="AC10" t="n">
-        <v>19</v>
-      </c>
-      <c r="AD10" t="inlineStr">
-        <is>
-          <t>The student explained the significance of Mendeleev's periodic table in organizing elements, predicting properties, and facilitating scientific understanding. The connection to nomenclature is accurate. The answer is thorough and demonstrates understanding.</t>
-        </is>
-      </c>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1941,49 +1595,12 @@
           <t>20240808047</t>
         </is>
       </c>
-      <c r="T11" t="n">
-        <v>63</v>
-      </c>
-      <c r="U11" t="n">
-        <v>10</v>
-      </c>
-      <c r="V11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student partially understands the role of chemistry in innovation and industrial progress, mentioning alchemy and the Dupont company. However, the answer lacks depth and precision regarding specific historical milestones and the collaborative aspects of chemistry's development. </t>
-        </is>
-      </c>
-      <c r="W11" t="n">
-        <v>18</v>
-      </c>
-      <c r="X11" t="inlineStr">
-        <is>
-          <t>The student correctly identifies that nomenclature helped eliminate pseudoscience and create a universal language for chemistry.  The answer is concise and accurate.</t>
-        </is>
-      </c>
-      <c r="Y11" t="n">
-        <v>5</v>
-      </c>
-      <c r="Z11" t="inlineStr">
-        <is>
-          <t>The student's answer is insufficient and does not offer valid alternatives to experimentation in chemical innovation. The response is circular and lacks substance.</t>
-        </is>
-      </c>
-      <c r="AA11" t="n">
-        <v>12</v>
-      </c>
-      <c r="AB11" t="inlineStr">
-        <is>
-          <t>The student lists several important instruments used in early chemistry, demonstrating basic knowledge of the tools used. However, the answer lacks detail or explanation of their significance.</t>
-        </is>
-      </c>
-      <c r="AC11" t="n">
-        <v>18</v>
-      </c>
-      <c r="AD11" t="inlineStr">
-        <is>
-          <t>The student correctly explains Mendeleev's organization of the periodic table and his prediction of new elements. This shows a good understanding of the significance of his work.</t>
-        </is>
-      </c>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2081,49 +1698,12 @@
           <t>20240809026</t>
         </is>
       </c>
-      <c r="T12" t="n">
-        <v>65</v>
-      </c>
-      <c r="U12" t="n">
-        <v>15</v>
-      </c>
-      <c r="V12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student correctly identifies Jabir ibn Hayyan and Antoine Lavoisier as important figures in the history of chemistry and provides a reasonable description of their contributions.  However, some claims are overstated or lack the necessary nuance.  For example,  calling Jabir 'the father of chemistry' is a simplification. </t>
-        </is>
-      </c>
-      <c r="W12" t="n">
-        <v>20</v>
-      </c>
-      <c r="X12" t="inlineStr">
-        <is>
-          <t>The student correctly explains that a universal nomenclature prevents confusion and enables scientific collaboration.</t>
-        </is>
-      </c>
-      <c r="Y12" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z12" t="inlineStr">
-        <is>
-          <t>The student's answer is partially correct in that theoretical work in chemistry is important, but it neglects the importance of experimental verification and practical application.  The statement is too simplistic.</t>
-        </is>
-      </c>
-      <c r="AA12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student's answer is insufficient and does not provide any relevant instruments/methods. </t>
-        </is>
-      </c>
-      <c r="AC12" t="n">
-        <v>20</v>
-      </c>
-      <c r="AD12" t="inlineStr">
-        <is>
-          <t>The student accurately describes the significance of Mendeleev's periodic table in classifying elements and predicting the properties of undiscovered ones.</t>
-        </is>
-      </c>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2221,49 +1801,12 @@
           <t>20230808074</t>
         </is>
       </c>
-      <c r="T13" t="n">
-        <v>65</v>
-      </c>
-      <c r="U13" t="n">
-        <v>10</v>
-      </c>
-      <c r="V13" t="inlineStr">
-        <is>
-          <t>The student demonstrates a basic understanding of Lavoisier's contribution to chemical nomenclature and the role of the chemical industry (DuPont). However, the description of the Karlsruhe Congress is inaccurate and incomplete, thus limiting the points received.</t>
-        </is>
-      </c>
-      <c r="W13" t="n">
-        <v>14</v>
-      </c>
-      <c r="X13" t="inlineStr">
-        <is>
-          <t>The student correctly identifies the importance of nomenclature for universal understanding and teaching.  The answer is well-articulated but lacks depth in exploring the specific ways nomenclature facilitates scientific collaboration and advancement.</t>
-        </is>
-      </c>
-      <c r="Y13" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z13" t="inlineStr">
-        <is>
-          <t>The student mentions Dalton's theoretical approach to chemistry, which is a valid alternative to purely experimental methods.  However, the explanation is limited and doesn't explore other potential alternatives or the interplay between theory and experiment.</t>
-        </is>
-      </c>
-      <c r="AA13" t="n">
-        <v>16</v>
-      </c>
-      <c r="AB13" t="inlineStr">
-        <is>
-          <t>The student correctly identifies and describes several important instruments in the development of chemistry (analytical balance, eudiometer, barometer, thermometer). The answer shows good understanding, but it could benefit from better connecting these instruments to specific advancements in chemical understanding.</t>
-        </is>
-      </c>
-      <c r="AC13" t="n">
-        <v>15</v>
-      </c>
-      <c r="AD13" t="inlineStr">
-        <is>
-          <t>The student accurately describes Mendeleev's prediction of undiscovered elements based on the periodic table. The answer is clear and concise but could be enhanced by discussing the broader impact of the periodic table on the organization and understanding of chemical elements.</t>
-        </is>
-      </c>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2361,49 +1904,12 @@
           <t>20230808021</t>
         </is>
       </c>
-      <c r="T14" t="n">
-        <v>52</v>
-      </c>
-      <c r="U14" t="n">
-        <v>10</v>
-      </c>
-      <c r="V14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student partially explains the importance of the periodic table and nomenclature in chemical innovation and collaboration.  However, the answer lacks depth and specific examples of milestones. </t>
-        </is>
-      </c>
-      <c r="W14" t="n">
-        <v>10</v>
-      </c>
-      <c r="X14" t="inlineStr">
-        <is>
-          <t>The student correctly points out that nomenclature improves the understandability and accessibility of scientific knowledge, thus accelerating scientific progress. However, the answer lacks detail and specific examples.</t>
-        </is>
-      </c>
-      <c r="Y14" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z14" t="inlineStr">
-        <is>
-          <t>The student focuses on nomenclature as an alternative to experiments for innovation, which is partially correct in terms of knowledge sharing. However, the answer overlooks other crucial aspects of chemical innovation, such as theoretical advancements and computational methods.</t>
-        </is>
-      </c>
-      <c r="AA14" t="n">
-        <v>12</v>
-      </c>
-      <c r="AB14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student lists several important instruments and their functions in the development of chemistry. However, the answer lacks discussion of their impact and significance, missing a deeper analysis of their role in shaping chemical understanding and progress. </t>
-        </is>
-      </c>
-      <c r="AC14" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student correctly identifies Mendeleev's contribution in organizing the elements, showing its impact on subsequent discoveries. However, the answer lacks detail regarding the predictive power of the periodic table and its broader implications for chemical theory. </t>
-        </is>
-      </c>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2501,49 +2007,12 @@
           <t>20230808050</t>
         </is>
       </c>
-      <c r="T15" t="n">
-        <v>73</v>
-      </c>
-      <c r="U15" t="n">
-        <v>10</v>
-      </c>
-      <c r="V15" t="inlineStr">
-        <is>
-          <t>The student correctly identified the Karlsruhe Conference as a milestone but needed to name a second and provide more detailed analysis for full points.</t>
-        </is>
-      </c>
-      <c r="W15" t="n">
-        <v>12</v>
-      </c>
-      <c r="X15" t="inlineStr">
-        <is>
-          <t>The student's response demonstrates understanding of nomenclature's role in scientific communication and development but lacks depth for full points.</t>
-        </is>
-      </c>
-      <c r="Y15" t="n">
-        <v>18</v>
-      </c>
-      <c r="Z15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The answer is accurate and provides relevant examples of alternative methods for innovation in chemistry beyond experimentation. </t>
-        </is>
-      </c>
-      <c r="AA15" t="n">
-        <v>15</v>
-      </c>
-      <c r="AB15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student lists several important instruments and methods but needs to elaborate on their specific impact for a higher score. </t>
-        </is>
-      </c>
-      <c r="AC15" t="n">
-        <v>18</v>
-      </c>
-      <c r="AD15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student accurately describes the significance of Mendeleev's Periodic Table and its impact on the prediction of new elements. </t>
-        </is>
-      </c>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2641,49 +2110,12 @@
           <t>20240808006</t>
         </is>
       </c>
-      <c r="T16" t="n">
-        <v>82</v>
-      </c>
-      <c r="U16" t="n">
-        <v>15</v>
-      </c>
-      <c r="V16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student correctly identifies Lavoisier's and Curie's contributions.  However, the explanation lacks depth and some parts are not directly related to the question. </t>
-        </is>
-      </c>
-      <c r="W16" t="n">
-        <v>20</v>
-      </c>
-      <c r="X16" t="inlineStr">
-        <is>
-          <t>The student's answer is correct and concisely explains the impact of nomenclature on the advancement of science.</t>
-        </is>
-      </c>
-      <c r="Y16" t="n">
-        <v>12</v>
-      </c>
-      <c r="Z16" t="inlineStr">
-        <is>
-          <t>The student provides alternative approaches to experimental innovation in chemistry, including lectures, funding, and organization of existing knowledge. The answer is partially correct and shows a basic understanding of different methods to advance chemistry</t>
-        </is>
-      </c>
-      <c r="AA16" t="n">
-        <v>15</v>
-      </c>
-      <c r="AB16" t="inlineStr">
-        <is>
-          <t>The student correctly identifies electrolysis and spectroscopes as pivotal instruments. The mention of crystallization is also relevant to early chemistry. However, more comprehensive details on their impact would improve the answer.</t>
-        </is>
-      </c>
-      <c r="AC16" t="n">
-        <v>20</v>
-      </c>
-      <c r="AD16" t="inlineStr">
-        <is>
-          <t>The student accurately describes Mendeleev's discovery of the periodic table's pattern based on atomic weight and his prediction of undiscovered elements.  The answer is complete and accurate.</t>
-        </is>
-      </c>
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
+      <c r="X16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2781,49 +2213,12 @@
           <t>20220808015</t>
         </is>
       </c>
-      <c r="T17" t="n">
-        <v>80</v>
-      </c>
-      <c r="U17" t="n">
-        <v>10</v>
-      </c>
-      <c r="V17" t="inlineStr">
-        <is>
-          <t>The student partially addressed the question by mentioning organic matter and radioactive elements. However, the answer lacks depth and specific examples of historical milestones in chemistry.</t>
-        </is>
-      </c>
-      <c r="W17" t="n">
-        <v>20</v>
-      </c>
-      <c r="X17" t="inlineStr">
-        <is>
-          <t>The student correctly explained the importance of nomenclature in creating a common language for scientists, facilitating communication and understanding across geographical boundaries.</t>
-        </is>
-      </c>
-      <c r="Y17" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z17" t="inlineStr">
-        <is>
-          <t>The student provided limited alternatives to experimentation by mentioning observations and literature reviews.  A more complete answer would have included other methods like computational modeling or theoretical analysis.</t>
-        </is>
-      </c>
-      <c r="AA17" t="n">
-        <v>20</v>
-      </c>
-      <c r="AB17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The student listed several important instruments and methods in chemistry, demonstrating a good understanding of practical techniques used throughout history. </t>
-        </is>
-      </c>
-      <c r="AC17" t="n">
-        <v>20</v>
-      </c>
-      <c r="AD17" t="inlineStr">
-        <is>
-          <t>The student accurately described Mendeleev's organization of the periodic table and its implications for the prediction of new elements.  The answer showcases understanding of the table's significance.</t>
-        </is>
-      </c>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+      <c r="X17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2927,11 +2322,6 @@
       <c r="W18" t="inlineStr"/>
       <c r="X18" t="inlineStr"/>
       <c r="Y18" t="inlineStr"/>
-      <c r="Z18" t="inlineStr"/>
-      <c r="AA18" t="inlineStr"/>
-      <c r="AB18" t="inlineStr"/>
-      <c r="AC18" t="inlineStr"/>
-      <c r="AD18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3035,11 +2425,6 @@
       <c r="W19" t="inlineStr"/>
       <c r="X19" t="inlineStr"/>
       <c r="Y19" t="inlineStr"/>
-      <c r="Z19" t="inlineStr"/>
-      <c r="AA19" t="inlineStr"/>
-      <c r="AB19" t="inlineStr"/>
-      <c r="AC19" t="inlineStr"/>
-      <c r="AD19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3143,11 +2528,6 @@
       <c r="W20" t="inlineStr"/>
       <c r="X20" t="inlineStr"/>
       <c r="Y20" t="inlineStr"/>
-      <c r="Z20" t="inlineStr"/>
-      <c r="AA20" t="inlineStr"/>
-      <c r="AB20" t="inlineStr"/>
-      <c r="AC20" t="inlineStr"/>
-      <c r="AD20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3251,11 +2631,6 @@
       <c r="W21" t="inlineStr"/>
       <c r="X21" t="inlineStr"/>
       <c r="Y21" t="inlineStr"/>
-      <c r="Z21" t="inlineStr"/>
-      <c r="AA21" t="inlineStr"/>
-      <c r="AB21" t="inlineStr"/>
-      <c r="AC21" t="inlineStr"/>
-      <c r="AD21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3359,11 +2734,6 @@
       <c r="W22" t="inlineStr"/>
       <c r="X22" t="inlineStr"/>
       <c r="Y22" t="inlineStr"/>
-      <c r="Z22" t="inlineStr"/>
-      <c r="AA22" t="inlineStr"/>
-      <c r="AB22" t="inlineStr"/>
-      <c r="AC22" t="inlineStr"/>
-      <c r="AD22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3467,11 +2837,6 @@
       <c r="W23" t="inlineStr"/>
       <c r="X23" t="inlineStr"/>
       <c r="Y23" t="inlineStr"/>
-      <c r="Z23" t="inlineStr"/>
-      <c r="AA23" t="inlineStr"/>
-      <c r="AB23" t="inlineStr"/>
-      <c r="AC23" t="inlineStr"/>
-      <c r="AD23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3575,11 +2940,6 @@
       <c r="W24" t="inlineStr"/>
       <c r="X24" t="inlineStr"/>
       <c r="Y24" t="inlineStr"/>
-      <c r="Z24" t="inlineStr"/>
-      <c r="AA24" t="inlineStr"/>
-      <c r="AB24" t="inlineStr"/>
-      <c r="AC24" t="inlineStr"/>
-      <c r="AD24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3683,11 +3043,6 @@
       <c r="W25" t="inlineStr"/>
       <c r="X25" t="inlineStr"/>
       <c r="Y25" t="inlineStr"/>
-      <c r="Z25" t="inlineStr"/>
-      <c r="AA25" t="inlineStr"/>
-      <c r="AB25" t="inlineStr"/>
-      <c r="AC25" t="inlineStr"/>
-      <c r="AD25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3791,11 +3146,6 @@
       <c r="W26" t="inlineStr"/>
       <c r="X26" t="inlineStr"/>
       <c r="Y26" t="inlineStr"/>
-      <c r="Z26" t="inlineStr"/>
-      <c r="AA26" t="inlineStr"/>
-      <c r="AB26" t="inlineStr"/>
-      <c r="AC26" t="inlineStr"/>
-      <c r="AD26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3899,11 +3249,6 @@
       <c r="W27" t="inlineStr"/>
       <c r="X27" t="inlineStr"/>
       <c r="Y27" t="inlineStr"/>
-      <c r="Z27" t="inlineStr"/>
-      <c r="AA27" t="inlineStr"/>
-      <c r="AB27" t="inlineStr"/>
-      <c r="AC27" t="inlineStr"/>
-      <c r="AD27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4007,11 +3352,6 @@
       <c r="W28" t="inlineStr"/>
       <c r="X28" t="inlineStr"/>
       <c r="Y28" t="inlineStr"/>
-      <c r="Z28" t="inlineStr"/>
-      <c r="AA28" t="inlineStr"/>
-      <c r="AB28" t="inlineStr"/>
-      <c r="AC28" t="inlineStr"/>
-      <c r="AD28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4115,11 +3455,6 @@
       <c r="W29" t="inlineStr"/>
       <c r="X29" t="inlineStr"/>
       <c r="Y29" t="inlineStr"/>
-      <c r="Z29" t="inlineStr"/>
-      <c r="AA29" t="inlineStr"/>
-      <c r="AB29" t="inlineStr"/>
-      <c r="AC29" t="inlineStr"/>
-      <c r="AD29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4223,11 +3558,6 @@
       <c r="W30" t="inlineStr"/>
       <c r="X30" t="inlineStr"/>
       <c r="Y30" t="inlineStr"/>
-      <c r="Z30" t="inlineStr"/>
-      <c r="AA30" t="inlineStr"/>
-      <c r="AB30" t="inlineStr"/>
-      <c r="AC30" t="inlineStr"/>
-      <c r="AD30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4331,11 +3661,6 @@
       <c r="W31" t="inlineStr"/>
       <c r="X31" t="inlineStr"/>
       <c r="Y31" t="inlineStr"/>
-      <c r="Z31" t="inlineStr"/>
-      <c r="AA31" t="inlineStr"/>
-      <c r="AB31" t="inlineStr"/>
-      <c r="AC31" t="inlineStr"/>
-      <c r="AD31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4439,11 +3764,6 @@
       <c r="W32" t="inlineStr"/>
       <c r="X32" t="inlineStr"/>
       <c r="Y32" t="inlineStr"/>
-      <c r="Z32" t="inlineStr"/>
-      <c r="AA32" t="inlineStr"/>
-      <c r="AB32" t="inlineStr"/>
-      <c r="AC32" t="inlineStr"/>
-      <c r="AD32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4547,11 +3867,6 @@
       <c r="W33" t="inlineStr"/>
       <c r="X33" t="inlineStr"/>
       <c r="Y33" t="inlineStr"/>
-      <c r="Z33" t="inlineStr"/>
-      <c r="AA33" t="inlineStr"/>
-      <c r="AB33" t="inlineStr"/>
-      <c r="AC33" t="inlineStr"/>
-      <c r="AD33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -4655,11 +3970,6 @@
       <c r="W34" t="inlineStr"/>
       <c r="X34" t="inlineStr"/>
       <c r="Y34" t="inlineStr"/>
-      <c r="Z34" t="inlineStr"/>
-      <c r="AA34" t="inlineStr"/>
-      <c r="AB34" t="inlineStr"/>
-      <c r="AC34" t="inlineStr"/>
-      <c r="AD34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4763,11 +4073,6 @@
       <c r="W35" t="inlineStr"/>
       <c r="X35" t="inlineStr"/>
       <c r="Y35" t="inlineStr"/>
-      <c r="Z35" t="inlineStr"/>
-      <c r="AA35" t="inlineStr"/>
-      <c r="AB35" t="inlineStr"/>
-      <c r="AC35" t="inlineStr"/>
-      <c r="AD35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4871,11 +4176,6 @@
       <c r="W36" t="inlineStr"/>
       <c r="X36" t="inlineStr"/>
       <c r="Y36" t="inlineStr"/>
-      <c r="Z36" t="inlineStr"/>
-      <c r="AA36" t="inlineStr"/>
-      <c r="AB36" t="inlineStr"/>
-      <c r="AC36" t="inlineStr"/>
-      <c r="AD36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4979,11 +4279,6 @@
       <c r="W37" t="inlineStr"/>
       <c r="X37" t="inlineStr"/>
       <c r="Y37" t="inlineStr"/>
-      <c r="Z37" t="inlineStr"/>
-      <c r="AA37" t="inlineStr"/>
-      <c r="AB37" t="inlineStr"/>
-      <c r="AC37" t="inlineStr"/>
-      <c r="AD37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -5087,11 +4382,6 @@
       <c r="W38" t="inlineStr"/>
       <c r="X38" t="inlineStr"/>
       <c r="Y38" t="inlineStr"/>
-      <c r="Z38" t="inlineStr"/>
-      <c r="AA38" t="inlineStr"/>
-      <c r="AB38" t="inlineStr"/>
-      <c r="AC38" t="inlineStr"/>
-      <c r="AD38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5195,11 +4485,6 @@
       <c r="W39" t="inlineStr"/>
       <c r="X39" t="inlineStr"/>
       <c r="Y39" t="inlineStr"/>
-      <c r="Z39" t="inlineStr"/>
-      <c r="AA39" t="inlineStr"/>
-      <c r="AB39" t="inlineStr"/>
-      <c r="AC39" t="inlineStr"/>
-      <c r="AD39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5303,11 +4588,6 @@
       <c r="W40" t="inlineStr"/>
       <c r="X40" t="inlineStr"/>
       <c r="Y40" t="inlineStr"/>
-      <c r="Z40" t="inlineStr"/>
-      <c r="AA40" t="inlineStr"/>
-      <c r="AB40" t="inlineStr"/>
-      <c r="AC40" t="inlineStr"/>
-      <c r="AD40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -5411,11 +4691,6 @@
       <c r="W41" t="inlineStr"/>
       <c r="X41" t="inlineStr"/>
       <c r="Y41" t="inlineStr"/>
-      <c r="Z41" t="inlineStr"/>
-      <c r="AA41" t="inlineStr"/>
-      <c r="AB41" t="inlineStr"/>
-      <c r="AC41" t="inlineStr"/>
-      <c r="AD41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -5519,11 +4794,6 @@
       <c r="W42" t="inlineStr"/>
       <c r="X42" t="inlineStr"/>
       <c r="Y42" t="inlineStr"/>
-      <c r="Z42" t="inlineStr"/>
-      <c r="AA42" t="inlineStr"/>
-      <c r="AB42" t="inlineStr"/>
-      <c r="AC42" t="inlineStr"/>
-      <c r="AD42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -5627,11 +4897,6 @@
       <c r="W43" t="inlineStr"/>
       <c r="X43" t="inlineStr"/>
       <c r="Y43" t="inlineStr"/>
-      <c r="Z43" t="inlineStr"/>
-      <c r="AA43" t="inlineStr"/>
-      <c r="AB43" t="inlineStr"/>
-      <c r="AC43" t="inlineStr"/>
-      <c r="AD43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -5731,11 +4996,6 @@
       <c r="W44" t="inlineStr"/>
       <c r="X44" t="inlineStr"/>
       <c r="Y44" t="inlineStr"/>
-      <c r="Z44" t="inlineStr"/>
-      <c r="AA44" t="inlineStr"/>
-      <c r="AB44" t="inlineStr"/>
-      <c r="AC44" t="inlineStr"/>
-      <c r="AD44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5839,11 +5099,6 @@
       <c r="W45" t="inlineStr"/>
       <c r="X45" t="inlineStr"/>
       <c r="Y45" t="inlineStr"/>
-      <c r="Z45" t="inlineStr"/>
-      <c r="AA45" t="inlineStr"/>
-      <c r="AB45" t="inlineStr"/>
-      <c r="AC45" t="inlineStr"/>
-      <c r="AD45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5947,11 +5202,6 @@
       <c r="W46" t="inlineStr"/>
       <c r="X46" t="inlineStr"/>
       <c r="Y46" t="inlineStr"/>
-      <c r="Z46" t="inlineStr"/>
-      <c r="AA46" t="inlineStr"/>
-      <c r="AB46" t="inlineStr"/>
-      <c r="AC46" t="inlineStr"/>
-      <c r="AD46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -6055,11 +5305,6 @@
       <c r="W47" t="inlineStr"/>
       <c r="X47" t="inlineStr"/>
       <c r="Y47" t="inlineStr"/>
-      <c r="Z47" t="inlineStr"/>
-      <c r="AA47" t="inlineStr"/>
-      <c r="AB47" t="inlineStr"/>
-      <c r="AC47" t="inlineStr"/>
-      <c r="AD47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -6163,11 +5408,6 @@
       <c r="W48" t="inlineStr"/>
       <c r="X48" t="inlineStr"/>
       <c r="Y48" t="inlineStr"/>
-      <c r="Z48" t="inlineStr"/>
-      <c r="AA48" t="inlineStr"/>
-      <c r="AB48" t="inlineStr"/>
-      <c r="AC48" t="inlineStr"/>
-      <c r="AD48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -6271,11 +5511,6 @@
       <c r="W49" t="inlineStr"/>
       <c r="X49" t="inlineStr"/>
       <c r="Y49" t="inlineStr"/>
-      <c r="Z49" t="inlineStr"/>
-      <c r="AA49" t="inlineStr"/>
-      <c r="AB49" t="inlineStr"/>
-      <c r="AC49" t="inlineStr"/>
-      <c r="AD49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -6379,11 +5614,6 @@
       <c r="W50" t="inlineStr"/>
       <c r="X50" t="inlineStr"/>
       <c r="Y50" t="inlineStr"/>
-      <c r="Z50" t="inlineStr"/>
-      <c r="AA50" t="inlineStr"/>
-      <c r="AB50" t="inlineStr"/>
-      <c r="AC50" t="inlineStr"/>
-      <c r="AD50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -6487,11 +5717,6 @@
       <c r="W51" t="inlineStr"/>
       <c r="X51" t="inlineStr"/>
       <c r="Y51" t="inlineStr"/>
-      <c r="Z51" t="inlineStr"/>
-      <c r="AA51" t="inlineStr"/>
-      <c r="AB51" t="inlineStr"/>
-      <c r="AC51" t="inlineStr"/>
-      <c r="AD51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -6595,11 +5820,6 @@
       <c r="W52" t="inlineStr"/>
       <c r="X52" t="inlineStr"/>
       <c r="Y52" t="inlineStr"/>
-      <c r="Z52" t="inlineStr"/>
-      <c r="AA52" t="inlineStr"/>
-      <c r="AB52" t="inlineStr"/>
-      <c r="AC52" t="inlineStr"/>
-      <c r="AD52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -6703,11 +5923,6 @@
       <c r="W53" t="inlineStr"/>
       <c r="X53" t="inlineStr"/>
       <c r="Y53" t="inlineStr"/>
-      <c r="Z53" t="inlineStr"/>
-      <c r="AA53" t="inlineStr"/>
-      <c r="AB53" t="inlineStr"/>
-      <c r="AC53" t="inlineStr"/>
-      <c r="AD53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -6811,11 +6026,6 @@
       <c r="W54" t="inlineStr"/>
       <c r="X54" t="inlineStr"/>
       <c r="Y54" t="inlineStr"/>
-      <c r="Z54" t="inlineStr"/>
-      <c r="AA54" t="inlineStr"/>
-      <c r="AB54" t="inlineStr"/>
-      <c r="AC54" t="inlineStr"/>
-      <c r="AD54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -6919,11 +6129,6 @@
       <c r="W55" t="inlineStr"/>
       <c r="X55" t="inlineStr"/>
       <c r="Y55" t="inlineStr"/>
-      <c r="Z55" t="inlineStr"/>
-      <c r="AA55" t="inlineStr"/>
-      <c r="AB55" t="inlineStr"/>
-      <c r="AC55" t="inlineStr"/>
-      <c r="AD55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -7027,11 +6232,6 @@
       <c r="W56" t="inlineStr"/>
       <c r="X56" t="inlineStr"/>
       <c r="Y56" t="inlineStr"/>
-      <c r="Z56" t="inlineStr"/>
-      <c r="AA56" t="inlineStr"/>
-      <c r="AB56" t="inlineStr"/>
-      <c r="AC56" t="inlineStr"/>
-      <c r="AD56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -7135,11 +6335,6 @@
       <c r="W57" t="inlineStr"/>
       <c r="X57" t="inlineStr"/>
       <c r="Y57" t="inlineStr"/>
-      <c r="Z57" t="inlineStr"/>
-      <c r="AA57" t="inlineStr"/>
-      <c r="AB57" t="inlineStr"/>
-      <c r="AC57" t="inlineStr"/>
-      <c r="AD57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -7243,11 +6438,6 @@
       <c r="W58" t="inlineStr"/>
       <c r="X58" t="inlineStr"/>
       <c r="Y58" t="inlineStr"/>
-      <c r="Z58" t="inlineStr"/>
-      <c r="AA58" t="inlineStr"/>
-      <c r="AB58" t="inlineStr"/>
-      <c r="AC58" t="inlineStr"/>
-      <c r="AD58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -7351,11 +6541,6 @@
       <c r="W59" t="inlineStr"/>
       <c r="X59" t="inlineStr"/>
       <c r="Y59" t="inlineStr"/>
-      <c r="Z59" t="inlineStr"/>
-      <c r="AA59" t="inlineStr"/>
-      <c r="AB59" t="inlineStr"/>
-      <c r="AC59" t="inlineStr"/>
-      <c r="AD59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -7459,11 +6644,6 @@
       <c r="W60" t="inlineStr"/>
       <c r="X60" t="inlineStr"/>
       <c r="Y60" t="inlineStr"/>
-      <c r="Z60" t="inlineStr"/>
-      <c r="AA60" t="inlineStr"/>
-      <c r="AB60" t="inlineStr"/>
-      <c r="AC60" t="inlineStr"/>
-      <c r="AD60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -7567,11 +6747,6 @@
       <c r="W61" t="inlineStr"/>
       <c r="X61" t="inlineStr"/>
       <c r="Y61" t="inlineStr"/>
-      <c r="Z61" t="inlineStr"/>
-      <c r="AA61" t="inlineStr"/>
-      <c r="AB61" t="inlineStr"/>
-      <c r="AC61" t="inlineStr"/>
-      <c r="AD61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -7675,11 +6850,6 @@
       <c r="W62" t="inlineStr"/>
       <c r="X62" t="inlineStr"/>
       <c r="Y62" t="inlineStr"/>
-      <c r="Z62" t="inlineStr"/>
-      <c r="AA62" t="inlineStr"/>
-      <c r="AB62" t="inlineStr"/>
-      <c r="AC62" t="inlineStr"/>
-      <c r="AD62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -7783,11 +6953,6 @@
       <c r="W63" t="inlineStr"/>
       <c r="X63" t="inlineStr"/>
       <c r="Y63" t="inlineStr"/>
-      <c r="Z63" t="inlineStr"/>
-      <c r="AA63" t="inlineStr"/>
-      <c r="AB63" t="inlineStr"/>
-      <c r="AC63" t="inlineStr"/>
-      <c r="AD63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -7891,11 +7056,6 @@
       <c r="W64" t="inlineStr"/>
       <c r="X64" t="inlineStr"/>
       <c r="Y64" t="inlineStr"/>
-      <c r="Z64" t="inlineStr"/>
-      <c r="AA64" t="inlineStr"/>
-      <c r="AB64" t="inlineStr"/>
-      <c r="AC64" t="inlineStr"/>
-      <c r="AD64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -7999,11 +7159,6 @@
       <c r="W65" t="inlineStr"/>
       <c r="X65" t="inlineStr"/>
       <c r="Y65" t="inlineStr"/>
-      <c r="Z65" t="inlineStr"/>
-      <c r="AA65" t="inlineStr"/>
-      <c r="AB65" t="inlineStr"/>
-      <c r="AC65" t="inlineStr"/>
-      <c r="AD65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -8107,11 +7262,6 @@
       <c r="W66" t="inlineStr"/>
       <c r="X66" t="inlineStr"/>
       <c r="Y66" t="inlineStr"/>
-      <c r="Z66" t="inlineStr"/>
-      <c r="AA66" t="inlineStr"/>
-      <c r="AB66" t="inlineStr"/>
-      <c r="AC66" t="inlineStr"/>
-      <c r="AD66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -8215,11 +7365,6 @@
       <c r="W67" t="inlineStr"/>
       <c r="X67" t="inlineStr"/>
       <c r="Y67" t="inlineStr"/>
-      <c r="Z67" t="inlineStr"/>
-      <c r="AA67" t="inlineStr"/>
-      <c r="AB67" t="inlineStr"/>
-      <c r="AC67" t="inlineStr"/>
-      <c r="AD67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -8323,11 +7468,6 @@
       <c r="W68" t="inlineStr"/>
       <c r="X68" t="inlineStr"/>
       <c r="Y68" t="inlineStr"/>
-      <c r="Z68" t="inlineStr"/>
-      <c r="AA68" t="inlineStr"/>
-      <c r="AB68" t="inlineStr"/>
-      <c r="AC68" t="inlineStr"/>
-      <c r="AD68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -8431,11 +7571,6 @@
       <c r="W69" t="inlineStr"/>
       <c r="X69" t="inlineStr"/>
       <c r="Y69" t="inlineStr"/>
-      <c r="Z69" t="inlineStr"/>
-      <c r="AA69" t="inlineStr"/>
-      <c r="AB69" t="inlineStr"/>
-      <c r="AC69" t="inlineStr"/>
-      <c r="AD69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -8539,11 +7674,6 @@
       <c r="W70" t="inlineStr"/>
       <c r="X70" t="inlineStr"/>
       <c r="Y70" t="inlineStr"/>
-      <c r="Z70" t="inlineStr"/>
-      <c r="AA70" t="inlineStr"/>
-      <c r="AB70" t="inlineStr"/>
-      <c r="AC70" t="inlineStr"/>
-      <c r="AD70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -8647,11 +7777,6 @@
       <c r="W71" t="inlineStr"/>
       <c r="X71" t="inlineStr"/>
       <c r="Y71" t="inlineStr"/>
-      <c r="Z71" t="inlineStr"/>
-      <c r="AA71" t="inlineStr"/>
-      <c r="AB71" t="inlineStr"/>
-      <c r="AC71" t="inlineStr"/>
-      <c r="AD71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -8755,11 +7880,6 @@
       <c r="W72" t="inlineStr"/>
       <c r="X72" t="inlineStr"/>
       <c r="Y72" t="inlineStr"/>
-      <c r="Z72" t="inlineStr"/>
-      <c r="AA72" t="inlineStr"/>
-      <c r="AB72" t="inlineStr"/>
-      <c r="AC72" t="inlineStr"/>
-      <c r="AD72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -8863,11 +7983,6 @@
       <c r="W73" t="inlineStr"/>
       <c r="X73" t="inlineStr"/>
       <c r="Y73" t="inlineStr"/>
-      <c r="Z73" t="inlineStr"/>
-      <c r="AA73" t="inlineStr"/>
-      <c r="AB73" t="inlineStr"/>
-      <c r="AC73" t="inlineStr"/>
-      <c r="AD73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -8971,11 +8086,6 @@
       <c r="W74" t="inlineStr"/>
       <c r="X74" t="inlineStr"/>
       <c r="Y74" t="inlineStr"/>
-      <c r="Z74" t="inlineStr"/>
-      <c r="AA74" t="inlineStr"/>
-      <c r="AB74" t="inlineStr"/>
-      <c r="AC74" t="inlineStr"/>
-      <c r="AD74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -9079,11 +8189,6 @@
       <c r="W75" t="inlineStr"/>
       <c r="X75" t="inlineStr"/>
       <c r="Y75" t="inlineStr"/>
-      <c r="Z75" t="inlineStr"/>
-      <c r="AA75" t="inlineStr"/>
-      <c r="AB75" t="inlineStr"/>
-      <c r="AC75" t="inlineStr"/>
-      <c r="AD75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -9187,11 +8292,6 @@
       <c r="W76" t="inlineStr"/>
       <c r="X76" t="inlineStr"/>
       <c r="Y76" t="inlineStr"/>
-      <c r="Z76" t="inlineStr"/>
-      <c r="AA76" t="inlineStr"/>
-      <c r="AB76" t="inlineStr"/>
-      <c r="AC76" t="inlineStr"/>
-      <c r="AD76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -9295,11 +8395,6 @@
       <c r="W77" t="inlineStr"/>
       <c r="X77" t="inlineStr"/>
       <c r="Y77" t="inlineStr"/>
-      <c r="Z77" t="inlineStr"/>
-      <c r="AA77" t="inlineStr"/>
-      <c r="AB77" t="inlineStr"/>
-      <c r="AC77" t="inlineStr"/>
-      <c r="AD77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -9403,11 +8498,6 @@
       <c r="W78" t="inlineStr"/>
       <c r="X78" t="inlineStr"/>
       <c r="Y78" t="inlineStr"/>
-      <c r="Z78" t="inlineStr"/>
-      <c r="AA78" t="inlineStr"/>
-      <c r="AB78" t="inlineStr"/>
-      <c r="AC78" t="inlineStr"/>
-      <c r="AD78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -9511,11 +8601,6 @@
       <c r="W79" t="inlineStr"/>
       <c r="X79" t="inlineStr"/>
       <c r="Y79" t="inlineStr"/>
-      <c r="Z79" t="inlineStr"/>
-      <c r="AA79" t="inlineStr"/>
-      <c r="AB79" t="inlineStr"/>
-      <c r="AC79" t="inlineStr"/>
-      <c r="AD79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -9619,11 +8704,6 @@
       <c r="W80" t="inlineStr"/>
       <c r="X80" t="inlineStr"/>
       <c r="Y80" t="inlineStr"/>
-      <c r="Z80" t="inlineStr"/>
-      <c r="AA80" t="inlineStr"/>
-      <c r="AB80" t="inlineStr"/>
-      <c r="AC80" t="inlineStr"/>
-      <c r="AD80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -9727,11 +8807,6 @@
       <c r="W81" t="inlineStr"/>
       <c r="X81" t="inlineStr"/>
       <c r="Y81" t="inlineStr"/>
-      <c r="Z81" t="inlineStr"/>
-      <c r="AA81" t="inlineStr"/>
-      <c r="AB81" t="inlineStr"/>
-      <c r="AC81" t="inlineStr"/>
-      <c r="AD81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -9835,11 +8910,6 @@
       <c r="W82" t="inlineStr"/>
       <c r="X82" t="inlineStr"/>
       <c r="Y82" t="inlineStr"/>
-      <c r="Z82" t="inlineStr"/>
-      <c r="AA82" t="inlineStr"/>
-      <c r="AB82" t="inlineStr"/>
-      <c r="AC82" t="inlineStr"/>
-      <c r="AD82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -9943,11 +9013,6 @@
       <c r="W83" t="inlineStr"/>
       <c r="X83" t="inlineStr"/>
       <c r="Y83" t="inlineStr"/>
-      <c r="Z83" t="inlineStr"/>
-      <c r="AA83" t="inlineStr"/>
-      <c r="AB83" t="inlineStr"/>
-      <c r="AC83" t="inlineStr"/>
-      <c r="AD83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -10051,11 +9116,6 @@
       <c r="W84" t="inlineStr"/>
       <c r="X84" t="inlineStr"/>
       <c r="Y84" t="inlineStr"/>
-      <c r="Z84" t="inlineStr"/>
-      <c r="AA84" t="inlineStr"/>
-      <c r="AB84" t="inlineStr"/>
-      <c r="AC84" t="inlineStr"/>
-      <c r="AD84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -10159,11 +9219,6 @@
       <c r="W85" t="inlineStr"/>
       <c r="X85" t="inlineStr"/>
       <c r="Y85" t="inlineStr"/>
-      <c r="Z85" t="inlineStr"/>
-      <c r="AA85" t="inlineStr"/>
-      <c r="AB85" t="inlineStr"/>
-      <c r="AC85" t="inlineStr"/>
-      <c r="AD85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -10267,11 +9322,6 @@
       <c r="W86" t="inlineStr"/>
       <c r="X86" t="inlineStr"/>
       <c r="Y86" t="inlineStr"/>
-      <c r="Z86" t="inlineStr"/>
-      <c r="AA86" t="inlineStr"/>
-      <c r="AB86" t="inlineStr"/>
-      <c r="AC86" t="inlineStr"/>
-      <c r="AD86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -10375,11 +9425,6 @@
       <c r="W87" t="inlineStr"/>
       <c r="X87" t="inlineStr"/>
       <c r="Y87" t="inlineStr"/>
-      <c r="Z87" t="inlineStr"/>
-      <c r="AA87" t="inlineStr"/>
-      <c r="AB87" t="inlineStr"/>
-      <c r="AC87" t="inlineStr"/>
-      <c r="AD87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -10483,11 +9528,6 @@
       <c r="W88" t="inlineStr"/>
       <c r="X88" t="inlineStr"/>
       <c r="Y88" t="inlineStr"/>
-      <c r="Z88" t="inlineStr"/>
-      <c r="AA88" t="inlineStr"/>
-      <c r="AB88" t="inlineStr"/>
-      <c r="AC88" t="inlineStr"/>
-      <c r="AD88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -10591,11 +9631,6 @@
       <c r="W89" t="inlineStr"/>
       <c r="X89" t="inlineStr"/>
       <c r="Y89" t="inlineStr"/>
-      <c r="Z89" t="inlineStr"/>
-      <c r="AA89" t="inlineStr"/>
-      <c r="AB89" t="inlineStr"/>
-      <c r="AC89" t="inlineStr"/>
-      <c r="AD89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -10699,11 +9734,6 @@
       <c r="W90" t="inlineStr"/>
       <c r="X90" t="inlineStr"/>
       <c r="Y90" t="inlineStr"/>
-      <c r="Z90" t="inlineStr"/>
-      <c r="AA90" t="inlineStr"/>
-      <c r="AB90" t="inlineStr"/>
-      <c r="AC90" t="inlineStr"/>
-      <c r="AD90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -10807,11 +9837,6 @@
       <c r="W91" t="inlineStr"/>
       <c r="X91" t="inlineStr"/>
       <c r="Y91" t="inlineStr"/>
-      <c r="Z91" t="inlineStr"/>
-      <c r="AA91" t="inlineStr"/>
-      <c r="AB91" t="inlineStr"/>
-      <c r="AC91" t="inlineStr"/>
-      <c r="AD91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -10915,11 +9940,6 @@
       <c r="W92" t="inlineStr"/>
       <c r="X92" t="inlineStr"/>
       <c r="Y92" t="inlineStr"/>
-      <c r="Z92" t="inlineStr"/>
-      <c r="AA92" t="inlineStr"/>
-      <c r="AB92" t="inlineStr"/>
-      <c r="AC92" t="inlineStr"/>
-      <c r="AD92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -11023,11 +10043,6 @@
       <c r="W93" t="inlineStr"/>
       <c r="X93" t="inlineStr"/>
       <c r="Y93" t="inlineStr"/>
-      <c r="Z93" t="inlineStr"/>
-      <c r="AA93" t="inlineStr"/>
-      <c r="AB93" t="inlineStr"/>
-      <c r="AC93" t="inlineStr"/>
-      <c r="AD93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -11131,11 +10146,6 @@
       <c r="W94" t="inlineStr"/>
       <c r="X94" t="inlineStr"/>
       <c r="Y94" t="inlineStr"/>
-      <c r="Z94" t="inlineStr"/>
-      <c r="AA94" t="inlineStr"/>
-      <c r="AB94" t="inlineStr"/>
-      <c r="AC94" t="inlineStr"/>
-      <c r="AD94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -11239,11 +10249,6 @@
       <c r="W95" t="inlineStr"/>
       <c r="X95" t="inlineStr"/>
       <c r="Y95" t="inlineStr"/>
-      <c r="Z95" t="inlineStr"/>
-      <c r="AA95" t="inlineStr"/>
-      <c r="AB95" t="inlineStr"/>
-      <c r="AC95" t="inlineStr"/>
-      <c r="AD95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -11347,11 +10352,6 @@
       <c r="W96" t="inlineStr"/>
       <c r="X96" t="inlineStr"/>
       <c r="Y96" t="inlineStr"/>
-      <c r="Z96" t="inlineStr"/>
-      <c r="AA96" t="inlineStr"/>
-      <c r="AB96" t="inlineStr"/>
-      <c r="AC96" t="inlineStr"/>
-      <c r="AD96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -11455,11 +10455,6 @@
       <c r="W97" t="inlineStr"/>
       <c r="X97" t="inlineStr"/>
       <c r="Y97" t="inlineStr"/>
-      <c r="Z97" t="inlineStr"/>
-      <c r="AA97" t="inlineStr"/>
-      <c r="AB97" t="inlineStr"/>
-      <c r="AC97" t="inlineStr"/>
-      <c r="AD97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -11563,11 +10558,6 @@
       <c r="W98" t="inlineStr"/>
       <c r="X98" t="inlineStr"/>
       <c r="Y98" t="inlineStr"/>
-      <c r="Z98" t="inlineStr"/>
-      <c r="AA98" t="inlineStr"/>
-      <c r="AB98" t="inlineStr"/>
-      <c r="AC98" t="inlineStr"/>
-      <c r="AD98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -11671,11 +10661,6 @@
       <c r="W99" t="inlineStr"/>
       <c r="X99" t="inlineStr"/>
       <c r="Y99" t="inlineStr"/>
-      <c r="Z99" t="inlineStr"/>
-      <c r="AA99" t="inlineStr"/>
-      <c r="AB99" t="inlineStr"/>
-      <c r="AC99" t="inlineStr"/>
-      <c r="AD99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -11779,11 +10764,6 @@
       <c r="W100" t="inlineStr"/>
       <c r="X100" t="inlineStr"/>
       <c r="Y100" t="inlineStr"/>
-      <c r="Z100" t="inlineStr"/>
-      <c r="AA100" t="inlineStr"/>
-      <c r="AB100" t="inlineStr"/>
-      <c r="AC100" t="inlineStr"/>
-      <c r="AD100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -11887,11 +10867,6 @@
       <c r="W101" t="inlineStr"/>
       <c r="X101" t="inlineStr"/>
       <c r="Y101" t="inlineStr"/>
-      <c r="Z101" t="inlineStr"/>
-      <c r="AA101" t="inlineStr"/>
-      <c r="AB101" t="inlineStr"/>
-      <c r="AC101" t="inlineStr"/>
-      <c r="AD101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -11995,11 +10970,6 @@
       <c r="W102" t="inlineStr"/>
       <c r="X102" t="inlineStr"/>
       <c r="Y102" t="inlineStr"/>
-      <c r="Z102" t="inlineStr"/>
-      <c r="AA102" t="inlineStr"/>
-      <c r="AB102" t="inlineStr"/>
-      <c r="AC102" t="inlineStr"/>
-      <c r="AD102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -12103,11 +11073,6 @@
       <c r="W103" t="inlineStr"/>
       <c r="X103" t="inlineStr"/>
       <c r="Y103" t="inlineStr"/>
-      <c r="Z103" t="inlineStr"/>
-      <c r="AA103" t="inlineStr"/>
-      <c r="AB103" t="inlineStr"/>
-      <c r="AC103" t="inlineStr"/>
-      <c r="AD103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -12211,11 +11176,6 @@
       <c r="W104" t="inlineStr"/>
       <c r="X104" t="inlineStr"/>
       <c r="Y104" t="inlineStr"/>
-      <c r="Z104" t="inlineStr"/>
-      <c r="AA104" t="inlineStr"/>
-      <c r="AB104" t="inlineStr"/>
-      <c r="AC104" t="inlineStr"/>
-      <c r="AD104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -12319,11 +11279,6 @@
       <c r="W105" t="inlineStr"/>
       <c r="X105" t="inlineStr"/>
       <c r="Y105" t="inlineStr"/>
-      <c r="Z105" t="inlineStr"/>
-      <c r="AA105" t="inlineStr"/>
-      <c r="AB105" t="inlineStr"/>
-      <c r="AC105" t="inlineStr"/>
-      <c r="AD105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -12427,11 +11382,6 @@
       <c r="W106" t="inlineStr"/>
       <c r="X106" t="inlineStr"/>
       <c r="Y106" t="inlineStr"/>
-      <c r="Z106" t="inlineStr"/>
-      <c r="AA106" t="inlineStr"/>
-      <c r="AB106" t="inlineStr"/>
-      <c r="AC106" t="inlineStr"/>
-      <c r="AD106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -12535,11 +11485,6 @@
       <c r="W107" t="inlineStr"/>
       <c r="X107" t="inlineStr"/>
       <c r="Y107" t="inlineStr"/>
-      <c r="Z107" t="inlineStr"/>
-      <c r="AA107" t="inlineStr"/>
-      <c r="AB107" t="inlineStr"/>
-      <c r="AC107" t="inlineStr"/>
-      <c r="AD107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -12643,11 +11588,6 @@
       <c r="W108" t="inlineStr"/>
       <c r="X108" t="inlineStr"/>
       <c r="Y108" t="inlineStr"/>
-      <c r="Z108" t="inlineStr"/>
-      <c r="AA108" t="inlineStr"/>
-      <c r="AB108" t="inlineStr"/>
-      <c r="AC108" t="inlineStr"/>
-      <c r="AD108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -12751,11 +11691,6 @@
       <c r="W109" t="inlineStr"/>
       <c r="X109" t="inlineStr"/>
       <c r="Y109" t="inlineStr"/>
-      <c r="Z109" t="inlineStr"/>
-      <c r="AA109" t="inlineStr"/>
-      <c r="AB109" t="inlineStr"/>
-      <c r="AC109" t="inlineStr"/>
-      <c r="AD109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -12859,11 +11794,6 @@
       <c r="W110" t="inlineStr"/>
       <c r="X110" t="inlineStr"/>
       <c r="Y110" t="inlineStr"/>
-      <c r="Z110" t="inlineStr"/>
-      <c r="AA110" t="inlineStr"/>
-      <c r="AB110" t="inlineStr"/>
-      <c r="AC110" t="inlineStr"/>
-      <c r="AD110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -12967,11 +11897,6 @@
       <c r="W111" t="inlineStr"/>
       <c r="X111" t="inlineStr"/>
       <c r="Y111" t="inlineStr"/>
-      <c r="Z111" t="inlineStr"/>
-      <c r="AA111" t="inlineStr"/>
-      <c r="AB111" t="inlineStr"/>
-      <c r="AC111" t="inlineStr"/>
-      <c r="AD111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -13075,11 +12000,6 @@
       <c r="W112" t="inlineStr"/>
       <c r="X112" t="inlineStr"/>
       <c r="Y112" t="inlineStr"/>
-      <c r="Z112" t="inlineStr"/>
-      <c r="AA112" t="inlineStr"/>
-      <c r="AB112" t="inlineStr"/>
-      <c r="AC112" t="inlineStr"/>
-      <c r="AD112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -13183,11 +12103,6 @@
       <c r="W113" t="inlineStr"/>
       <c r="X113" t="inlineStr"/>
       <c r="Y113" t="inlineStr"/>
-      <c r="Z113" t="inlineStr"/>
-      <c r="AA113" t="inlineStr"/>
-      <c r="AB113" t="inlineStr"/>
-      <c r="AC113" t="inlineStr"/>
-      <c r="AD113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -13291,11 +12206,6 @@
       <c r="W114" t="inlineStr"/>
       <c r="X114" t="inlineStr"/>
       <c r="Y114" t="inlineStr"/>
-      <c r="Z114" t="inlineStr"/>
-      <c r="AA114" t="inlineStr"/>
-      <c r="AB114" t="inlineStr"/>
-      <c r="AC114" t="inlineStr"/>
-      <c r="AD114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -13399,11 +12309,6 @@
       <c r="W115" t="inlineStr"/>
       <c r="X115" t="inlineStr"/>
       <c r="Y115" t="inlineStr"/>
-      <c r="Z115" t="inlineStr"/>
-      <c r="AA115" t="inlineStr"/>
-      <c r="AB115" t="inlineStr"/>
-      <c r="AC115" t="inlineStr"/>
-      <c r="AD115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -13507,11 +12412,6 @@
       <c r="W116" t="inlineStr"/>
       <c r="X116" t="inlineStr"/>
       <c r="Y116" t="inlineStr"/>
-      <c r="Z116" t="inlineStr"/>
-      <c r="AA116" t="inlineStr"/>
-      <c r="AB116" t="inlineStr"/>
-      <c r="AC116" t="inlineStr"/>
-      <c r="AD116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -13615,11 +12515,6 @@
       <c r="W117" t="inlineStr"/>
       <c r="X117" t="inlineStr"/>
       <c r="Y117" t="inlineStr"/>
-      <c r="Z117" t="inlineStr"/>
-      <c r="AA117" t="inlineStr"/>
-      <c r="AB117" t="inlineStr"/>
-      <c r="AC117" t="inlineStr"/>
-      <c r="AD117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -13723,11 +12618,6 @@
       <c r="W118" t="inlineStr"/>
       <c r="X118" t="inlineStr"/>
       <c r="Y118" t="inlineStr"/>
-      <c r="Z118" t="inlineStr"/>
-      <c r="AA118" t="inlineStr"/>
-      <c r="AB118" t="inlineStr"/>
-      <c r="AC118" t="inlineStr"/>
-      <c r="AD118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -13831,11 +12721,6 @@
       <c r="W119" t="inlineStr"/>
       <c r="X119" t="inlineStr"/>
       <c r="Y119" t="inlineStr"/>
-      <c r="Z119" t="inlineStr"/>
-      <c r="AA119" t="inlineStr"/>
-      <c r="AB119" t="inlineStr"/>
-      <c r="AC119" t="inlineStr"/>
-      <c r="AD119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -13939,11 +12824,6 @@
       <c r="W120" t="inlineStr"/>
       <c r="X120" t="inlineStr"/>
       <c r="Y120" t="inlineStr"/>
-      <c r="Z120" t="inlineStr"/>
-      <c r="AA120" t="inlineStr"/>
-      <c r="AB120" t="inlineStr"/>
-      <c r="AC120" t="inlineStr"/>
-      <c r="AD120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -14047,11 +12927,6 @@
       <c r="W121" t="inlineStr"/>
       <c r="X121" t="inlineStr"/>
       <c r="Y121" t="inlineStr"/>
-      <c r="Z121" t="inlineStr"/>
-      <c r="AA121" t="inlineStr"/>
-      <c r="AB121" t="inlineStr"/>
-      <c r="AC121" t="inlineStr"/>
-      <c r="AD121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -14155,11 +13030,6 @@
       <c r="W122" t="inlineStr"/>
       <c r="X122" t="inlineStr"/>
       <c r="Y122" t="inlineStr"/>
-      <c r="Z122" t="inlineStr"/>
-      <c r="AA122" t="inlineStr"/>
-      <c r="AB122" t="inlineStr"/>
-      <c r="AC122" t="inlineStr"/>
-      <c r="AD122" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>